<commit_message>
working on final report
</commit_message>
<xml_diff>
--- a/3d scanner accuracy.xlsx
+++ b/3d scanner accuracy.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab PC\Documents\GitHub\crumple_curvature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956E12BD-84EA-4AD4-9BF3-47172AC878B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631B37AB-91E5-42FD-96DD-952ADEEAA67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{DBF9DEE0-FB45-4EDB-A912-0D186C42FD17}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{DBF9DEE0-FB45-4EDB-A912-0D186C42FD17}"/>
   </bookViews>
   <sheets>
     <sheet name="READ_ME" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Spheres" sheetId="3" r:id="rId3"/>
+    <sheet name="5insphere" sheetId="4" r:id="rId4"/>
+    <sheet name="Scurve" sheetId="5" r:id="rId5"/>
+    <sheet name="cylindrical sheet" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="253">
   <si>
     <t>measured</t>
   </si>
@@ -912,6 +916,39 @@
   <si>
     <t>high resolution scan lapLACIAN SMOOTH 1 iterations Poisson simpication to .3% of original size</t>
   </si>
+  <si>
+    <t>Scruv</t>
+  </si>
+  <si>
+    <t>Calculated gaussian curvature with the STL file</t>
+  </si>
+  <si>
+    <t>Gaussian curvature of the same file but resampled to 10% of original size</t>
+  </si>
+  <si>
+    <t>Average Gaussian Curvature</t>
+  </si>
+  <si>
+    <t>Standard Devation</t>
+  </si>
+  <si>
+    <t>Filtered Average Gaussian Curvature</t>
+  </si>
+  <si>
+    <t>50% sampled</t>
+  </si>
+  <si>
+    <t>30% sampled</t>
+  </si>
+  <si>
+    <t>10% sampled</t>
+  </si>
+  <si>
+    <t>simplied 50%</t>
+  </si>
+  <si>
+    <t>Theoretical curvatue</t>
+  </si>
 </sst>
 </file>
 
@@ -921,7 +958,7 @@
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -986,6 +1023,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA709F5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1647,7 +1690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1819,16 +1862,100 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1882,113 +2009,19 @@
     <xf numFmtId="11" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2006,6 +2039,368 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>480629</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>91843</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB2C1504-685A-DD42-B1B4-5F4046EC5049}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9768840" y="190500"/>
+          <a:ext cx="6561389" cy="4656223"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>305353</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>160447</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E8AC77A-757C-52B5-4F4F-3641A71D1730}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9776460" y="5105400"/>
+          <a:ext cx="6378493" cy="4930567"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>807719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>126412</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11D566F8-EEBA-442E-B7D1-50CBAF2D65BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6492240" y="3916679"/>
+          <a:ext cx="3528060" cy="3235373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>138973</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7DD4623-3F90-40A9-BD99-13A92C6FF5AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3291840"/>
+          <a:ext cx="3040380" cy="3247933"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>643355</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>160359</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E95A6D61-630D-6069-0F41-74F4BEB51FD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="4008120"/>
+          <a:ext cx="4148554" cy="3177879"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>701041</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>54865</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63F53013-4F30-7A06-9640-A6F311DB1CBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4152901" y="4015740"/>
+          <a:ext cx="3956304" cy="3169920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>68581</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>77930</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>23197</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F51ED84E-CC41-3331-115E-B5F2E87CF9F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8122921" y="3994610"/>
+          <a:ext cx="4084319" cy="3237107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>716281</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>125859</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13281105-7CBD-049A-AA98-28B3081BD65E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12222481" y="3977640"/>
+          <a:ext cx="4012058" cy="3269320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2307,604 +2702,605 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E9F438A-EE7A-4EB3-A371-6D123C01379F}">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L41"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R31" activeCellId="1" sqref="S4 R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="109" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
+      <c r="A2" s="109"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
+      <c r="A3" s="109"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="99"/>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
+      <c r="A4" s="109"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="99"/>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
+      <c r="A5" s="109"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="109"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="99"/>
-      <c r="B6" s="99"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="99"/>
+      <c r="A6" s="109"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="99"/>
-      <c r="B7" s="99"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
+      <c r="A7" s="109"/>
+      <c r="B7" s="109"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="109"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="109"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="99"/>
-      <c r="B8" s="99"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99"/>
+      <c r="A8" s="109"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="109"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="109"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="99"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="99"/>
-      <c r="L9" s="99"/>
+      <c r="A9" s="109"/>
+      <c r="B9" s="109"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="109"/>
+      <c r="K9" s="109"/>
+      <c r="L9" s="109"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="99"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="99"/>
-      <c r="J10" s="99"/>
-      <c r="K10" s="99"/>
-      <c r="L10" s="99"/>
+      <c r="A10" s="109"/>
+      <c r="B10" s="109"/>
+      <c r="C10" s="109"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="109"/>
+      <c r="K10" s="109"/>
+      <c r="L10" s="109"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="99"/>
-      <c r="B11" s="99"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="99"/>
-      <c r="J11" s="99"/>
-      <c r="K11" s="99"/>
-      <c r="L11" s="99"/>
+      <c r="A11" s="109"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="109"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="109"/>
+      <c r="K11" s="109"/>
+      <c r="L11" s="109"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="99"/>
-      <c r="B12" s="99"/>
-      <c r="C12" s="99"/>
-      <c r="D12" s="99"/>
-      <c r="E12" s="99"/>
-      <c r="F12" s="99"/>
-      <c r="G12" s="99"/>
-      <c r="H12" s="99"/>
-      <c r="I12" s="99"/>
-      <c r="J12" s="99"/>
-      <c r="K12" s="99"/>
-      <c r="L12" s="99"/>
+      <c r="A12" s="109"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="109"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="109"/>
+      <c r="K12" s="109"/>
+      <c r="L12" s="109"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="99"/>
-      <c r="B13" s="99"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="99"/>
-      <c r="J13" s="99"/>
-      <c r="K13" s="99"/>
-      <c r="L13" s="99"/>
+      <c r="A13" s="109"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="109"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="109"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="109"/>
+      <c r="K13" s="109"/>
+      <c r="L13" s="109"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="99"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="99"/>
-      <c r="D14" s="99"/>
-      <c r="E14" s="99"/>
-      <c r="F14" s="99"/>
-      <c r="G14" s="99"/>
-      <c r="H14" s="99"/>
-      <c r="I14" s="99"/>
-      <c r="J14" s="99"/>
-      <c r="K14" s="99"/>
-      <c r="L14" s="99"/>
+      <c r="A14" s="109"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="109"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="109"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="99"/>
-      <c r="B15" s="99"/>
-      <c r="C15" s="99"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="99"/>
-      <c r="F15" s="99"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="99"/>
-      <c r="J15" s="99"/>
-      <c r="K15" s="99"/>
-      <c r="L15" s="99"/>
+      <c r="A15" s="109"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="109"/>
+      <c r="K15" s="109"/>
+      <c r="L15" s="109"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="99"/>
-      <c r="B16" s="99"/>
-      <c r="C16" s="99"/>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="99"/>
+      <c r="A16" s="109"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="109"/>
+      <c r="F16" s="109"/>
+      <c r="G16" s="109"/>
+      <c r="H16" s="109"/>
+      <c r="I16" s="109"/>
+      <c r="J16" s="109"/>
+      <c r="K16" s="109"/>
+      <c r="L16" s="109"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="99"/>
-      <c r="B17" s="99"/>
-      <c r="C17" s="99"/>
-      <c r="D17" s="99"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="99"/>
-      <c r="G17" s="99"/>
-      <c r="H17" s="99"/>
-      <c r="I17" s="99"/>
-      <c r="J17" s="99"/>
-      <c r="K17" s="99"/>
-      <c r="L17" s="99"/>
+      <c r="A17" s="109"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="109"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="109"/>
+      <c r="K17" s="109"/>
+      <c r="L17" s="109"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="99"/>
-      <c r="B18" s="99"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="99"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="99"/>
-      <c r="I18" s="99"/>
-      <c r="J18" s="99"/>
-      <c r="K18" s="99"/>
-      <c r="L18" s="99"/>
+      <c r="A18" s="109"/>
+      <c r="B18" s="109"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
+      <c r="G18" s="109"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="109"/>
+      <c r="K18" s="109"/>
+      <c r="L18" s="109"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="99"/>
-      <c r="B19" s="99"/>
-      <c r="C19" s="99"/>
-      <c r="D19" s="99"/>
-      <c r="E19" s="99"/>
-      <c r="F19" s="99"/>
-      <c r="G19" s="99"/>
-      <c r="H19" s="99"/>
-      <c r="I19" s="99"/>
-      <c r="J19" s="99"/>
-      <c r="K19" s="99"/>
-      <c r="L19" s="99"/>
+      <c r="A19" s="109"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="109"/>
+      <c r="G19" s="109"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="109"/>
+      <c r="K19" s="109"/>
+      <c r="L19" s="109"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="99"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="99"/>
-      <c r="I20" s="99"/>
-      <c r="J20" s="99"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="99"/>
+      <c r="A20" s="109"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="109"/>
+      <c r="G20" s="109"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="109"/>
+      <c r="J20" s="109"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="109"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="99"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="99"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="99"/>
-      <c r="J21" s="99"/>
-      <c r="K21" s="99"/>
-      <c r="L21" s="99"/>
+      <c r="A21" s="109"/>
+      <c r="B21" s="109"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
+      <c r="J21" s="109"/>
+      <c r="K21" s="109"/>
+      <c r="L21" s="109"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="99"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="99"/>
-      <c r="D22" s="99"/>
-      <c r="E22" s="99"/>
-      <c r="F22" s="99"/>
-      <c r="G22" s="99"/>
-      <c r="H22" s="99"/>
-      <c r="I22" s="99"/>
-      <c r="J22" s="99"/>
-      <c r="K22" s="99"/>
-      <c r="L22" s="99"/>
+      <c r="A22" s="109"/>
+      <c r="B22" s="109"/>
+      <c r="C22" s="109"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="109"/>
+      <c r="F22" s="109"/>
+      <c r="G22" s="109"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="109"/>
+      <c r="J22" s="109"/>
+      <c r="K22" s="109"/>
+      <c r="L22" s="109"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="99"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="99"/>
-      <c r="D23" s="99"/>
-      <c r="E23" s="99"/>
-      <c r="F23" s="99"/>
-      <c r="G23" s="99"/>
-      <c r="H23" s="99"/>
-      <c r="I23" s="99"/>
-      <c r="J23" s="99"/>
-      <c r="K23" s="99"/>
-      <c r="L23" s="99"/>
+      <c r="A23" s="109"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="109"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="109"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="109"/>
+      <c r="J23" s="109"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="109"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="99"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="99"/>
-      <c r="D24" s="99"/>
-      <c r="E24" s="99"/>
-      <c r="F24" s="99"/>
-      <c r="G24" s="99"/>
-      <c r="H24" s="99"/>
-      <c r="I24" s="99"/>
-      <c r="J24" s="99"/>
-      <c r="K24" s="99"/>
-      <c r="L24" s="99"/>
+      <c r="A24" s="109"/>
+      <c r="B24" s="109"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="109"/>
+      <c r="G24" s="109"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="109"/>
+      <c r="J24" s="109"/>
+      <c r="K24" s="109"/>
+      <c r="L24" s="109"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="99"/>
-      <c r="B25" s="99"/>
-      <c r="C25" s="99"/>
-      <c r="D25" s="99"/>
-      <c r="E25" s="99"/>
-      <c r="F25" s="99"/>
-      <c r="G25" s="99"/>
-      <c r="H25" s="99"/>
-      <c r="I25" s="99"/>
-      <c r="J25" s="99"/>
-      <c r="K25" s="99"/>
-      <c r="L25" s="99"/>
+      <c r="A25" s="109"/>
+      <c r="B25" s="109"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="109"/>
+      <c r="H25" s="109"/>
+      <c r="I25" s="109"/>
+      <c r="J25" s="109"/>
+      <c r="K25" s="109"/>
+      <c r="L25" s="109"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="99"/>
-      <c r="B26" s="99"/>
-      <c r="C26" s="99"/>
-      <c r="D26" s="99"/>
-      <c r="E26" s="99"/>
-      <c r="F26" s="99"/>
-      <c r="G26" s="99"/>
-      <c r="H26" s="99"/>
-      <c r="I26" s="99"/>
-      <c r="J26" s="99"/>
-      <c r="K26" s="99"/>
-      <c r="L26" s="99"/>
+      <c r="A26" s="109"/>
+      <c r="B26" s="109"/>
+      <c r="C26" s="109"/>
+      <c r="D26" s="109"/>
+      <c r="E26" s="109"/>
+      <c r="F26" s="109"/>
+      <c r="G26" s="109"/>
+      <c r="H26" s="109"/>
+      <c r="I26" s="109"/>
+      <c r="J26" s="109"/>
+      <c r="K26" s="109"/>
+      <c r="L26" s="109"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="99"/>
-      <c r="B27" s="99"/>
-      <c r="C27" s="99"/>
-      <c r="D27" s="99"/>
-      <c r="E27" s="99"/>
-      <c r="F27" s="99"/>
-      <c r="G27" s="99"/>
-      <c r="H27" s="99"/>
-      <c r="I27" s="99"/>
-      <c r="J27" s="99"/>
-      <c r="K27" s="99"/>
-      <c r="L27" s="99"/>
+      <c r="A27" s="109"/>
+      <c r="B27" s="109"/>
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="109"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="109"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="99"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="99"/>
-      <c r="D28" s="99"/>
-      <c r="E28" s="99"/>
-      <c r="F28" s="99"/>
-      <c r="G28" s="99"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="99"/>
-      <c r="J28" s="99"/>
-      <c r="K28" s="99"/>
-      <c r="L28" s="99"/>
+      <c r="A28" s="109"/>
+      <c r="B28" s="109"/>
+      <c r="C28" s="109"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="109"/>
+      <c r="G28" s="109"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="109"/>
+      <c r="J28" s="109"/>
+      <c r="K28" s="109"/>
+      <c r="L28" s="109"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="99"/>
-      <c r="B29" s="99"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="99"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="99"/>
-      <c r="J29" s="99"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="99"/>
+      <c r="A29" s="109"/>
+      <c r="B29" s="109"/>
+      <c r="C29" s="109"/>
+      <c r="D29" s="109"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="109"/>
+      <c r="G29" s="109"/>
+      <c r="H29" s="109"/>
+      <c r="I29" s="109"/>
+      <c r="J29" s="109"/>
+      <c r="K29" s="109"/>
+      <c r="L29" s="109"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="99"/>
-      <c r="B30" s="99"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="99"/>
-      <c r="F30" s="99"/>
-      <c r="G30" s="99"/>
-      <c r="H30" s="99"/>
-      <c r="I30" s="99"/>
-      <c r="J30" s="99"/>
-      <c r="K30" s="99"/>
-      <c r="L30" s="99"/>
+      <c r="A30" s="109"/>
+      <c r="B30" s="109"/>
+      <c r="C30" s="109"/>
+      <c r="D30" s="109"/>
+      <c r="E30" s="109"/>
+      <c r="F30" s="109"/>
+      <c r="G30" s="109"/>
+      <c r="H30" s="109"/>
+      <c r="I30" s="109"/>
+      <c r="J30" s="109"/>
+      <c r="K30" s="109"/>
+      <c r="L30" s="109"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="99"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="99"/>
-      <c r="J31" s="99"/>
-      <c r="K31" s="99"/>
-      <c r="L31" s="99"/>
+      <c r="A31" s="109"/>
+      <c r="B31" s="109"/>
+      <c r="C31" s="109"/>
+      <c r="D31" s="109"/>
+      <c r="E31" s="109"/>
+      <c r="F31" s="109"/>
+      <c r="G31" s="109"/>
+      <c r="H31" s="109"/>
+      <c r="I31" s="109"/>
+      <c r="J31" s="109"/>
+      <c r="K31" s="109"/>
+      <c r="L31" s="109"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="99"/>
-      <c r="B32" s="99"/>
-      <c r="C32" s="99"/>
-      <c r="D32" s="99"/>
-      <c r="E32" s="99"/>
-      <c r="F32" s="99"/>
-      <c r="G32" s="99"/>
-      <c r="H32" s="99"/>
-      <c r="I32" s="99"/>
-      <c r="J32" s="99"/>
-      <c r="K32" s="99"/>
-      <c r="L32" s="99"/>
+      <c r="A32" s="109"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="109"/>
+      <c r="D32" s="109"/>
+      <c r="E32" s="109"/>
+      <c r="F32" s="109"/>
+      <c r="G32" s="109"/>
+      <c r="H32" s="109"/>
+      <c r="I32" s="109"/>
+      <c r="J32" s="109"/>
+      <c r="K32" s="109"/>
+      <c r="L32" s="109"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="99"/>
-      <c r="B33" s="99"/>
-      <c r="C33" s="99"/>
-      <c r="D33" s="99"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="99"/>
-      <c r="G33" s="99"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="99"/>
-      <c r="K33" s="99"/>
-      <c r="L33" s="99"/>
+      <c r="A33" s="109"/>
+      <c r="B33" s="109"/>
+      <c r="C33" s="109"/>
+      <c r="D33" s="109"/>
+      <c r="E33" s="109"/>
+      <c r="F33" s="109"/>
+      <c r="G33" s="109"/>
+      <c r="H33" s="109"/>
+      <c r="I33" s="109"/>
+      <c r="J33" s="109"/>
+      <c r="K33" s="109"/>
+      <c r="L33" s="109"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="99"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="99"/>
-      <c r="D34" s="99"/>
-      <c r="E34" s="99"/>
-      <c r="F34" s="99"/>
-      <c r="G34" s="99"/>
-      <c r="H34" s="99"/>
-      <c r="I34" s="99"/>
-      <c r="J34" s="99"/>
-      <c r="K34" s="99"/>
-      <c r="L34" s="99"/>
+      <c r="A34" s="109"/>
+      <c r="B34" s="109"/>
+      <c r="C34" s="109"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="109"/>
+      <c r="J34" s="109"/>
+      <c r="K34" s="109"/>
+      <c r="L34" s="109"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="99"/>
-      <c r="B35" s="99"/>
-      <c r="C35" s="99"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="99"/>
-      <c r="F35" s="99"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="99"/>
-      <c r="J35" s="99"/>
-      <c r="K35" s="99"/>
-      <c r="L35" s="99"/>
+      <c r="A35" s="109"/>
+      <c r="B35" s="109"/>
+      <c r="C35" s="109"/>
+      <c r="D35" s="109"/>
+      <c r="E35" s="109"/>
+      <c r="F35" s="109"/>
+      <c r="G35" s="109"/>
+      <c r="H35" s="109"/>
+      <c r="I35" s="109"/>
+      <c r="J35" s="109"/>
+      <c r="K35" s="109"/>
+      <c r="L35" s="109"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="99"/>
-      <c r="B36" s="99"/>
-      <c r="C36" s="99"/>
-      <c r="D36" s="99"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="99"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="99"/>
-      <c r="K36" s="99"/>
-      <c r="L36" s="99"/>
+      <c r="A36" s="109"/>
+      <c r="B36" s="109"/>
+      <c r="C36" s="109"/>
+      <c r="D36" s="109"/>
+      <c r="E36" s="109"/>
+      <c r="F36" s="109"/>
+      <c r="G36" s="109"/>
+      <c r="H36" s="109"/>
+      <c r="I36" s="109"/>
+      <c r="J36" s="109"/>
+      <c r="K36" s="109"/>
+      <c r="L36" s="109"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="99"/>
-      <c r="B37" s="99"/>
-      <c r="C37" s="99"/>
-      <c r="D37" s="99"/>
-      <c r="E37" s="99"/>
-      <c r="F37" s="99"/>
-      <c r="G37" s="99"/>
-      <c r="H37" s="99"/>
-      <c r="I37" s="99"/>
-      <c r="J37" s="99"/>
-      <c r="K37" s="99"/>
-      <c r="L37" s="99"/>
+      <c r="A37" s="109"/>
+      <c r="B37" s="109"/>
+      <c r="C37" s="109"/>
+      <c r="D37" s="109"/>
+      <c r="E37" s="109"/>
+      <c r="F37" s="109"/>
+      <c r="G37" s="109"/>
+      <c r="H37" s="109"/>
+      <c r="I37" s="109"/>
+      <c r="J37" s="109"/>
+      <c r="K37" s="109"/>
+      <c r="L37" s="109"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="99"/>
-      <c r="B38" s="99"/>
-      <c r="C38" s="99"/>
-      <c r="D38" s="99"/>
-      <c r="E38" s="99"/>
-      <c r="F38" s="99"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="99"/>
-      <c r="I38" s="99"/>
-      <c r="J38" s="99"/>
-      <c r="K38" s="99"/>
-      <c r="L38" s="99"/>
+      <c r="A38" s="109"/>
+      <c r="B38" s="109"/>
+      <c r="C38" s="109"/>
+      <c r="D38" s="109"/>
+      <c r="E38" s="109"/>
+      <c r="F38" s="109"/>
+      <c r="G38" s="109"/>
+      <c r="H38" s="109"/>
+      <c r="I38" s="109"/>
+      <c r="J38" s="109"/>
+      <c r="K38" s="109"/>
+      <c r="L38" s="109"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="99"/>
-      <c r="B39" s="99"/>
-      <c r="C39" s="99"/>
-      <c r="D39" s="99"/>
-      <c r="E39" s="99"/>
-      <c r="F39" s="99"/>
-      <c r="G39" s="99"/>
-      <c r="H39" s="99"/>
-      <c r="I39" s="99"/>
-      <c r="J39" s="99"/>
-      <c r="K39" s="99"/>
-      <c r="L39" s="99"/>
+      <c r="A39" s="109"/>
+      <c r="B39" s="109"/>
+      <c r="C39" s="109"/>
+      <c r="D39" s="109"/>
+      <c r="E39" s="109"/>
+      <c r="F39" s="109"/>
+      <c r="G39" s="109"/>
+      <c r="H39" s="109"/>
+      <c r="I39" s="109"/>
+      <c r="J39" s="109"/>
+      <c r="K39" s="109"/>
+      <c r="L39" s="109"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="99"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="99"/>
-      <c r="F40" s="99"/>
-      <c r="G40" s="99"/>
-      <c r="H40" s="99"/>
-      <c r="I40" s="99"/>
-      <c r="J40" s="99"/>
-      <c r="K40" s="99"/>
-      <c r="L40" s="99"/>
+      <c r="A40" s="109"/>
+      <c r="B40" s="109"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="109"/>
+      <c r="E40" s="109"/>
+      <c r="F40" s="109"/>
+      <c r="G40" s="109"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="109"/>
+      <c r="J40" s="109"/>
+      <c r="K40" s="109"/>
+      <c r="L40" s="109"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="99"/>
-      <c r="B41" s="99"/>
-      <c r="C41" s="99"/>
-      <c r="D41" s="99"/>
-      <c r="E41" s="99"/>
-      <c r="F41" s="99"/>
-      <c r="G41" s="99"/>
-      <c r="H41" s="99"/>
-      <c r="I41" s="99"/>
-      <c r="J41" s="99"/>
-      <c r="K41" s="99"/>
-      <c r="L41" s="99"/>
+      <c r="A41" s="109"/>
+      <c r="B41" s="109"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="109"/>
+      <c r="F41" s="109"/>
+      <c r="G41" s="109"/>
+      <c r="H41" s="109"/>
+      <c r="I41" s="109"/>
+      <c r="J41" s="109"/>
+      <c r="K41" s="109"/>
+      <c r="L41" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A04D1E7-A26C-43E7-BA3E-95F23209ECBF}">
-  <dimension ref="A1:BQ121"/>
+  <dimension ref="A1:BQ118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A31" sqref="A31"/>
-      <selection pane="topRight" activeCell="Y108" sqref="Y108"/>
+      <selection pane="topRight" activeCell="S127" sqref="S127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3026,20 +3422,20 @@
       <c r="A10" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="99" t="s">
+      <c r="C10" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="99"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="99"/>
-      <c r="J10" s="99"/>
-      <c r="K10" s="99"/>
-      <c r="L10" s="99"/>
-      <c r="M10" s="99"/>
-      <c r="N10" s="99"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="109"/>
+      <c r="K10" s="109"/>
+      <c r="L10" s="109"/>
+      <c r="M10" s="109"/>
+      <c r="N10" s="109"/>
     </row>
     <row r="11" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="74">
@@ -3047,14 +3443,14 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="105" t="s">
+      <c r="E11" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="106"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106"/>
-      <c r="J11" s="107"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
+      <c r="H11" s="136"/>
+      <c r="I11" s="136"/>
+      <c r="J11" s="137"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
@@ -3352,13 +3748,13 @@
         <v>27</v>
       </c>
       <c r="S33" s="5"/>
-      <c r="AD33" s="108" t="s">
+      <c r="AD33" s="138" t="s">
         <v>59</v>
       </c>
-      <c r="AE33" s="108"/>
-      <c r="AF33" s="108"/>
-      <c r="AG33" s="108"/>
-      <c r="AH33" s="108"/>
+      <c r="AE33" s="138"/>
+      <c r="AF33" s="138"/>
+      <c r="AG33" s="138"/>
+      <c r="AH33" s="138"/>
     </row>
     <row r="34" spans="1:66" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
@@ -4288,14 +4684,14 @@
       <c r="AH45" s="3"/>
     </row>
     <row r="46" spans="1:66" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="109" t="s">
+      <c r="A46" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="109"/>
-      <c r="C46" s="109"/>
-      <c r="D46" s="109"/>
-      <c r="E46" s="109"/>
-      <c r="F46" s="109"/>
+      <c r="B46" s="139"/>
+      <c r="C46" s="139"/>
+      <c r="D46" s="139"/>
+      <c r="E46" s="139"/>
+      <c r="F46" s="139"/>
       <c r="G46" s="36"/>
       <c r="H46" s="36"/>
       <c r="I46" s="36"/>
@@ -4314,30 +4710,30 @@
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
-      <c r="Y46" s="115" t="s">
+      <c r="Y46" s="145" t="s">
         <v>125</v>
       </c>
-      <c r="Z46" s="116"/>
-      <c r="AA46" s="116"/>
-      <c r="AB46" s="116"/>
-      <c r="AC46" s="117" t="s">
+      <c r="Z46" s="146"/>
+      <c r="AA46" s="146"/>
+      <c r="AB46" s="146"/>
+      <c r="AC46" s="147" t="s">
         <v>128</v>
       </c>
-      <c r="AD46" s="117"/>
-      <c r="AE46" s="117"/>
-      <c r="AF46" s="117"/>
+      <c r="AD46" s="147"/>
+      <c r="AE46" s="147"/>
+      <c r="AF46" s="147"/>
       <c r="AI46" s="3"/>
     </row>
     <row r="47" spans="1:66" ht="101.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A47" s="73"/>
-      <c r="B47" s="110" t="s">
+      <c r="B47" s="140" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="111"/>
-      <c r="D47" s="111"/>
-      <c r="E47" s="111"/>
-      <c r="F47" s="111"/>
-      <c r="G47" s="112"/>
+      <c r="C47" s="141"/>
+      <c r="D47" s="141"/>
+      <c r="E47" s="141"/>
+      <c r="F47" s="141"/>
+      <c r="G47" s="142"/>
       <c r="H47" s="36" t="s">
         <v>97</v>
       </c>
@@ -4357,69 +4753,69 @@
       <c r="V47" s="36"/>
       <c r="W47" s="36"/>
       <c r="X47" s="3"/>
-      <c r="Y47" s="113" t="s">
+      <c r="Y47" s="143" t="s">
         <v>121</v>
       </c>
-      <c r="Z47" s="114"/>
-      <c r="AA47" s="114"/>
-      <c r="AB47" s="114"/>
-      <c r="AC47" s="114" t="s">
+      <c r="Z47" s="144"/>
+      <c r="AA47" s="144"/>
+      <c r="AB47" s="144"/>
+      <c r="AC47" s="144" t="s">
         <v>127</v>
       </c>
-      <c r="AD47" s="114"/>
-      <c r="AE47" s="114"/>
-      <c r="AF47" s="114"/>
-      <c r="AG47" s="118" t="s">
+      <c r="AD47" s="144"/>
+      <c r="AE47" s="144"/>
+      <c r="AF47" s="144"/>
+      <c r="AG47" s="148" t="s">
         <v>138</v>
       </c>
-      <c r="AH47" s="118"/>
-      <c r="AI47" s="118"/>
-      <c r="AJ47" s="118"/>
-      <c r="AK47" s="118"/>
-      <c r="AL47" s="118"/>
-      <c r="AM47" s="118"/>
-      <c r="AN47" s="118"/>
-      <c r="AO47" s="119"/>
-      <c r="AP47" s="120" t="s">
+      <c r="AH47" s="148"/>
+      <c r="AI47" s="148"/>
+      <c r="AJ47" s="148"/>
+      <c r="AK47" s="148"/>
+      <c r="AL47" s="148"/>
+      <c r="AM47" s="148"/>
+      <c r="AN47" s="148"/>
+      <c r="AO47" s="149"/>
+      <c r="AP47" s="126" t="s">
         <v>147</v>
       </c>
-      <c r="AQ47" s="121"/>
-      <c r="AR47" s="122"/>
+      <c r="AQ47" s="127"/>
+      <c r="AR47" s="128"/>
       <c r="AS47" s="58" t="s">
         <v>145</v>
       </c>
       <c r="AT47" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="AU47" s="129" t="s">
+      <c r="AU47" s="110" t="s">
         <v>152</v>
       </c>
-      <c r="AV47" s="130"/>
-      <c r="AW47" s="131"/>
-      <c r="AX47" s="129" t="s">
+      <c r="AV47" s="111"/>
+      <c r="AW47" s="112"/>
+      <c r="AX47" s="110" t="s">
         <v>153</v>
       </c>
-      <c r="AY47" s="130"/>
-      <c r="AZ47" s="131"/>
-      <c r="BA47" s="129" t="s">
+      <c r="AY47" s="111"/>
+      <c r="AZ47" s="112"/>
+      <c r="BA47" s="110" t="s">
         <v>158</v>
       </c>
-      <c r="BB47" s="130"/>
-      <c r="BC47" s="142"/>
-      <c r="BD47" s="134" t="s">
+      <c r="BB47" s="111"/>
+      <c r="BC47" s="119"/>
+      <c r="BD47" s="131" t="s">
         <v>165</v>
       </c>
-      <c r="BE47" s="135"/>
-      <c r="BF47" s="135"/>
-      <c r="BG47" s="135"/>
-      <c r="BI47" s="99" t="s">
+      <c r="BE47" s="132"/>
+      <c r="BF47" s="132"/>
+      <c r="BG47" s="132"/>
+      <c r="BI47" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="BJ47" s="99"/>
-      <c r="BK47" s="99"/>
-      <c r="BL47" s="99"/>
-      <c r="BM47" s="99"/>
-      <c r="BN47" s="99"/>
+      <c r="BJ47" s="109"/>
+      <c r="BK47" s="109"/>
+      <c r="BL47" s="109"/>
+      <c r="BM47" s="109"/>
+      <c r="BN47" s="109"/>
     </row>
     <row r="48" spans="1:66" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="75"/>
@@ -6192,28 +6588,28 @@
     </row>
     <row r="57" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E57" s="3"/>
-      <c r="AP57" s="123" t="s">
+      <c r="AP57" s="120" t="s">
         <v>144</v>
       </c>
-      <c r="AQ57" s="124"/>
-      <c r="AR57" s="125"/>
+      <c r="AQ57" s="121"/>
+      <c r="AR57" s="122"/>
       <c r="AS57" s="1"/>
       <c r="AT57" s="1"/>
-      <c r="AU57" s="123" t="s">
+      <c r="AU57" s="120" t="s">
         <v>151</v>
       </c>
-      <c r="AV57" s="124"/>
-      <c r="AW57" s="132"/>
-      <c r="AX57" s="136" t="s">
+      <c r="AV57" s="121"/>
+      <c r="AW57" s="129"/>
+      <c r="AX57" s="113" t="s">
         <v>157</v>
       </c>
-      <c r="AY57" s="137"/>
-      <c r="AZ57" s="138"/>
-      <c r="BA57" s="123" t="s">
+      <c r="AY57" s="114"/>
+      <c r="AZ57" s="115"/>
+      <c r="BA57" s="120" t="s">
         <v>163</v>
       </c>
-      <c r="BB57" s="124"/>
-      <c r="BC57" s="125"/>
+      <c r="BB57" s="121"/>
+      <c r="BC57" s="122"/>
       <c r="BD57" s="94"/>
       <c r="BE57" s="95"/>
       <c r="BF57" s="95"/>
@@ -6225,20 +6621,20 @@
         <f>51/81</f>
         <v>0.62962962962962965</v>
       </c>
-      <c r="AP58" s="126"/>
-      <c r="AQ58" s="127"/>
-      <c r="AR58" s="128"/>
+      <c r="AP58" s="123"/>
+      <c r="AQ58" s="124"/>
+      <c r="AR58" s="125"/>
       <c r="AS58" s="1"/>
       <c r="AT58" s="1"/>
-      <c r="AU58" s="126"/>
-      <c r="AV58" s="127"/>
-      <c r="AW58" s="133"/>
-      <c r="AX58" s="139"/>
-      <c r="AY58" s="140"/>
-      <c r="AZ58" s="141"/>
-      <c r="BA58" s="126"/>
-      <c r="BB58" s="127"/>
-      <c r="BC58" s="128"/>
+      <c r="AU58" s="123"/>
+      <c r="AV58" s="124"/>
+      <c r="AW58" s="130"/>
+      <c r="AX58" s="116"/>
+      <c r="AY58" s="117"/>
+      <c r="AZ58" s="118"/>
+      <c r="BA58" s="123"/>
+      <c r="BB58" s="124"/>
+      <c r="BC58" s="125"/>
       <c r="BD58" s="89"/>
       <c r="BE58" s="89"/>
       <c r="BF58" s="89"/>
@@ -6259,19 +6655,19 @@
       <c r="G62" s="4"/>
     </row>
     <row r="63" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="103" t="s">
+      <c r="A63" s="133" t="s">
         <v>70</v>
       </c>
-      <c r="B63" s="104"/>
-      <c r="C63" s="104"/>
-      <c r="D63" s="104"/>
-      <c r="E63" s="104"/>
-      <c r="F63" s="104"/>
-      <c r="G63" s="104"/>
-      <c r="H63" s="104"/>
-      <c r="I63" s="104"/>
-      <c r="J63" s="104"/>
-      <c r="K63" s="104"/>
+      <c r="B63" s="134"/>
+      <c r="C63" s="134"/>
+      <c r="D63" s="134"/>
+      <c r="E63" s="134"/>
+      <c r="F63" s="134"/>
+      <c r="G63" s="134"/>
+      <c r="H63" s="134"/>
+      <c r="I63" s="134"/>
+      <c r="J63" s="134"/>
+      <c r="K63" s="134"/>
     </row>
     <row r="64" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A64" s="33"/>
@@ -6492,39 +6888,39 @@
       </c>
     </row>
     <row r="70" spans="1:19" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="101" t="s">
+      <c r="B70" s="151" t="s">
         <v>187</v>
       </c>
-      <c r="C70" s="102"/>
-      <c r="D70" s="102"/>
-      <c r="E70" s="102"/>
-      <c r="F70" s="102"/>
-      <c r="G70" s="102"/>
+      <c r="C70" s="152"/>
+      <c r="D70" s="152"/>
+      <c r="E70" s="152"/>
+      <c r="F70" s="152"/>
+      <c r="G70" s="152"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B72" s="100" t="s">
+      <c r="B72" s="150" t="s">
         <v>186</v>
       </c>
-      <c r="C72" s="99"/>
-      <c r="D72" s="99"/>
-      <c r="E72" s="99"/>
-      <c r="F72" s="99"/>
-      <c r="G72" s="99"/>
-      <c r="I72" s="99" t="s">
+      <c r="C72" s="109"/>
+      <c r="D72" s="109"/>
+      <c r="E72" s="109"/>
+      <c r="F72" s="109"/>
+      <c r="G72" s="109"/>
+      <c r="I72" s="109" t="s">
         <v>188</v>
       </c>
-      <c r="J72" s="99"/>
-      <c r="K72" s="99"/>
-      <c r="L72" s="99"/>
-      <c r="M72" s="99"/>
-      <c r="N72" s="99"/>
-      <c r="O72" s="99" t="s">
+      <c r="J72" s="109"/>
+      <c r="K72" s="109"/>
+      <c r="L72" s="109"/>
+      <c r="M72" s="109"/>
+      <c r="N72" s="109"/>
+      <c r="O72" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="P72" s="99"/>
-      <c r="Q72" s="99"/>
-      <c r="R72" s="99"/>
-      <c r="S72" s="99"/>
+      <c r="P72" s="109"/>
+      <c r="Q72" s="109"/>
+      <c r="R72" s="109"/>
+      <c r="S72" s="109"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="74" t="s">
@@ -6653,71 +7049,71 @@
       <c r="A76" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="C76" s="144">
+      <c r="C76" s="99">
         <f>ABS($B$74-C75)/($B$74)*100</f>
         <v>27.597419354838703</v>
       </c>
-      <c r="D76" s="144">
+      <c r="D76" s="99">
         <f t="shared" ref="D76:S76" si="9">ABS($B$74-D75)/($B$74)*100</f>
         <v>14.07741935483871</v>
       </c>
-      <c r="E76" s="144">
+      <c r="E76" s="99">
         <f t="shared" si="9"/>
         <v>9.9329032258064576</v>
       </c>
-      <c r="F76" s="144">
+      <c r="F76" s="99">
         <f t="shared" si="9"/>
         <v>2.6864516129032339</v>
       </c>
-      <c r="G76" s="144">
+      <c r="G76" s="99">
         <f t="shared" si="9"/>
         <v>5.0064516129032359</v>
       </c>
-      <c r="H76" s="144">
+      <c r="H76" s="99">
         <f t="shared" si="9"/>
         <v>4.7870967741935457</v>
       </c>
-      <c r="I76" s="144">
+      <c r="I76" s="99">
         <f t="shared" si="9"/>
         <v>1.587096774193552</v>
       </c>
-      <c r="J76" s="144">
+      <c r="J76" s="99">
         <f t="shared" si="9"/>
         <v>0.23483870967740969</v>
       </c>
-      <c r="K76" s="144">
+      <c r="K76" s="99">
         <f t="shared" si="9"/>
         <v>0.36387096774192895</v>
       </c>
-      <c r="L76" s="144">
+      <c r="L76" s="99">
         <f t="shared" si="9"/>
         <v>4.0438709677419267</v>
       </c>
-      <c r="M76" s="144">
+      <c r="M76" s="99">
         <f t="shared" si="9"/>
         <v>3.5741935483870932</v>
       </c>
-      <c r="N76" s="144">
+      <c r="N76" s="99">
         <f t="shared" si="9"/>
         <v>8.516129032257852E-2</v>
       </c>
-      <c r="O76" s="144">
+      <c r="O76" s="99">
         <f t="shared" si="9"/>
         <v>2.8051612903225829</v>
       </c>
-      <c r="P76" s="144">
+      <c r="P76" s="99">
         <f t="shared" si="9"/>
         <v>1.5896774193548409</v>
       </c>
-      <c r="Q76" s="144">
+      <c r="Q76" s="99">
         <f t="shared" si="9"/>
         <v>4.3251612903225798</v>
       </c>
-      <c r="R76" s="144">
+      <c r="R76" s="99">
         <f t="shared" si="9"/>
         <v>1.4787096774193447</v>
       </c>
-      <c r="S76" s="144">
+      <c r="S76" s="99">
         <f t="shared" si="9"/>
         <v>1.6645161290322497</v>
       </c>
@@ -6782,71 +7178,71 @@
       <c r="A78" s="74" t="s">
         <v>198</v>
       </c>
-      <c r="C78" s="143">
+      <c r="C78">
         <f>(C77/C75)*100</f>
         <v>9445.3949244368396</v>
       </c>
-      <c r="D78" s="143">
+      <c r="D78">
         <f t="shared" ref="D78:G78" si="10">(D77/D75)*100</f>
         <v>1628.7750254496095</v>
       </c>
-      <c r="E78" s="143">
+      <c r="E78">
         <f t="shared" si="10"/>
         <v>1150.2617432334091</v>
       </c>
-      <c r="F78" s="143">
+      <c r="F78">
         <f t="shared" si="10"/>
         <v>1156.0403106230051</v>
       </c>
-      <c r="G78" s="143">
+      <c r="G78">
         <f t="shared" si="10"/>
         <v>368.64094372081593</v>
       </c>
-      <c r="H78" s="143">
+      <c r="H78">
         <f t="shared" ref="H78" si="11">(H77/H75)*100</f>
         <v>86.147174413877224</v>
       </c>
-      <c r="I78" s="143">
+      <c r="I78">
         <f t="shared" ref="I78" si="12">(I77/I75)*100</f>
         <v>82.32185951987806</v>
       </c>
-      <c r="J78" s="143">
+      <c r="J78">
         <f t="shared" ref="J78:K78" si="13">(J77/J75)*100</f>
         <v>68.757598489355644</v>
       </c>
-      <c r="K78" s="143">
+      <c r="K78">
         <f t="shared" si="13"/>
         <v>87.129943795488103</v>
       </c>
-      <c r="L78" s="143">
+      <c r="L78">
         <f t="shared" ref="L78" si="14">(L77/L75)*100</f>
         <v>48.705053384611247</v>
       </c>
-      <c r="M78" s="143">
+      <c r="M78">
         <f t="shared" ref="M78" si="15">(M77/M75)*100</f>
         <v>37.144386457915161</v>
       </c>
-      <c r="N78" s="143">
+      <c r="N78">
         <f t="shared" ref="N78:O78" si="16">(N77/N75)*100</f>
         <v>9.8254389809968288</v>
       </c>
-      <c r="O78" s="143">
+      <c r="O78">
         <f t="shared" si="16"/>
         <v>82.871783978971408</v>
       </c>
-      <c r="P78" s="143">
+      <c r="P78">
         <f t="shared" ref="P78" si="17">(P77/P75)*100</f>
         <v>62.408873970734781</v>
       </c>
-      <c r="Q78" s="143">
+      <c r="Q78">
         <f t="shared" ref="Q78" si="18">(Q77/Q75)*100</f>
         <v>57.862653072233918</v>
       </c>
-      <c r="R78" s="143">
+      <c r="R78">
         <f t="shared" ref="R78:S78" si="19">(R77/R75)*100</f>
         <v>43.41095423946355</v>
       </c>
-      <c r="S78" s="143">
+      <c r="S78">
         <f t="shared" si="19"/>
         <v>35.071512924813014</v>
       </c>
@@ -7101,71 +7497,71 @@
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C84" s="144">
+      <c r="C84" s="99">
         <f>ABS($B$82-C83)/($B$82)*100</f>
         <v>2.1669085631349811</v>
       </c>
-      <c r="D84" s="144">
+      <c r="D84" s="99">
         <f t="shared" ref="D84:S84" si="20">ABS($B$82-D83)/($B$82)*100</f>
         <v>6.8345428156749</v>
       </c>
-      <c r="E84" s="144">
+      <c r="E84" s="99">
         <f t="shared" si="20"/>
         <v>3.957910014513776</v>
       </c>
-      <c r="F84" s="144">
+      <c r="F84" s="99">
         <f t="shared" si="20"/>
         <v>1.8142235123367088</v>
       </c>
-      <c r="G84" s="144">
+      <c r="G84" s="99">
         <f t="shared" si="20"/>
         <v>1.0899854862118954</v>
       </c>
-      <c r="H84" s="144">
+      <c r="H84" s="99">
         <f t="shared" si="20"/>
         <v>1.2902757619738601</v>
       </c>
-      <c r="I84" s="144">
+      <c r="I84" s="99">
         <f t="shared" si="20"/>
         <v>0.67634252539912509</v>
       </c>
-      <c r="J84" s="144">
+      <c r="J84" s="99">
         <f t="shared" si="20"/>
         <v>0.18432510885341757</v>
       </c>
-      <c r="K84" s="144">
+      <c r="K84" s="99">
         <f t="shared" si="20"/>
         <v>1.0986937590711228</v>
       </c>
-      <c r="L84" s="144">
+      <c r="L84" s="99">
         <f t="shared" si="20"/>
         <v>0.93613933236574265</v>
       </c>
-      <c r="M84" s="144">
+      <c r="M84" s="99">
         <f t="shared" si="20"/>
         <v>0.31204644412190374</v>
       </c>
-      <c r="N84" s="144">
+      <c r="N84" s="99">
         <f t="shared" si="20"/>
         <v>0.7735849056603622</v>
       </c>
-      <c r="O84" s="144">
+      <c r="O84" s="99">
         <f t="shared" si="20"/>
         <v>1.0420899854862231</v>
       </c>
-      <c r="P84" s="144">
+      <c r="P84" s="99">
         <f t="shared" si="20"/>
         <v>0.21335268505080579</v>
       </c>
-      <c r="Q84" s="144">
+      <c r="Q84" s="99">
         <f t="shared" si="20"/>
         <v>4.6444121915827447E-2</v>
       </c>
-      <c r="R84" s="144">
+      <c r="R84" s="99">
         <f t="shared" si="20"/>
         <v>0.30333817126269197</v>
       </c>
-      <c r="S84" s="144">
+      <c r="S84" s="99">
         <f t="shared" si="20"/>
         <v>9.5791001451376409E-2</v>
       </c>
@@ -7230,71 +7626,71 @@
       <c r="A86" s="74" t="s">
         <v>198</v>
       </c>
-      <c r="C86" s="143">
+      <c r="C86">
         <f>(C85/C83)*100</f>
         <v>1186.820359903274</v>
       </c>
-      <c r="D86" s="143">
+      <c r="D86">
         <f t="shared" ref="D86:S86" si="21">(D85/D83)*100</f>
         <v>794.50390241622665</v>
       </c>
-      <c r="E86" s="143">
+      <c r="E86">
         <f t="shared" si="21"/>
         <v>432.79768802267301</v>
       </c>
-      <c r="F86" s="143">
+      <c r="F86">
         <f t="shared" si="21"/>
         <v>370.63435495367071</v>
       </c>
-      <c r="G86" s="143">
+      <c r="G86">
         <f t="shared" si="21"/>
         <v>186.6448435772638</v>
       </c>
-      <c r="H86" s="143">
+      <c r="H86">
         <f t="shared" si="21"/>
         <v>49.076502027540158</v>
       </c>
-      <c r="I86" s="143">
+      <c r="I86">
         <f t="shared" si="21"/>
         <v>66.516737306461366</v>
       </c>
-      <c r="J86" s="143">
+      <c r="J86">
         <f t="shared" si="21"/>
         <v>48.631003446119848</v>
       </c>
-      <c r="K86" s="143">
+      <c r="K86">
         <f t="shared" si="21"/>
         <v>45.620239789853692</v>
       </c>
-      <c r="L86" s="143">
+      <c r="L86">
         <f t="shared" si="21"/>
         <v>35.344021856352001</v>
       </c>
-      <c r="M86" s="143">
+      <c r="M86">
         <f t="shared" si="21"/>
         <v>26.114446936265644</v>
       </c>
-      <c r="N86" s="143">
+      <c r="N86">
         <f t="shared" si="21"/>
         <v>9.348436622355365</v>
       </c>
-      <c r="O86" s="143">
+      <c r="O86">
         <f t="shared" si="21"/>
         <v>62.454900120266345</v>
       </c>
-      <c r="P86" s="143">
+      <c r="P86">
         <f t="shared" si="21"/>
         <v>45.102031911334777</v>
       </c>
-      <c r="Q86" s="143">
+      <c r="Q86">
         <f t="shared" si="21"/>
         <v>36.986699192658421</v>
       </c>
-      <c r="R86" s="143">
+      <c r="R86">
         <f t="shared" si="21"/>
         <v>29.514245612004224</v>
       </c>
-      <c r="S86" s="143">
+      <c r="S86">
         <f t="shared" si="21"/>
         <v>23.069338514630395</v>
       </c>
@@ -7550,71 +7946,71 @@
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C92">
-        <f>ABS($B$90-C91)/($B$90)*100</f>
+        <f t="shared" ref="C92:S92" si="22">ABS($B$90-C91)/($B$90)*100</f>
         <v>3.2258064516128977</v>
       </c>
       <c r="D92">
-        <f>ABS($B$90-D91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516128977</v>
       </c>
       <c r="E92">
-        <f>ABS($B$90-E91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516128977</v>
       </c>
       <c r="F92">
-        <f>ABS($B$90-F91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516128977</v>
       </c>
       <c r="G92">
-        <f>ABS($B$90-G91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="H92">
-        <f>ABS($B$90-H91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="I92">
-        <f>ABS($B$90-I91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="J92">
-        <f>ABS($B$90-J91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="K92">
-        <f>ABS($B$90-K91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="L92">
-        <f>ABS($B$90-L91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="M92">
-        <f>ABS($B$90-M91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="N92">
-        <f>ABS($B$90-N91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="O92">
-        <f>ABS($B$90-O91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516128977</v>
       </c>
       <c r="P92">
-        <f>ABS($B$90-P91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516128977</v>
       </c>
       <c r="Q92">
-        <f>ABS($B$90-Q91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516128977</v>
       </c>
       <c r="R92">
-        <f>ABS($B$90-R91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516128977</v>
       </c>
       <c r="S92">
-        <f>ABS($B$90-S91)/($B$90)*100</f>
+        <f t="shared" si="22"/>
         <v>3.2258064516129115</v>
       </c>
     </row>
@@ -7683,67 +8079,67 @@
         <v>293.33333333333337</v>
       </c>
       <c r="D94">
-        <f t="shared" ref="D94:S94" si="22">(D93/D91)*100</f>
+        <f t="shared" ref="D94:S94" si="23">(D93/D91)*100</f>
         <v>200</v>
       </c>
       <c r="E94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>186.66666666666666</v>
       </c>
       <c r="F94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>166.66666666666669</v>
       </c>
       <c r="G94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>87.5</v>
       </c>
       <c r="H94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>29.665000000000003</v>
       </c>
       <c r="I94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>53.396875000000001</v>
       </c>
       <c r="J94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>36.281874999999999</v>
       </c>
       <c r="K94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>33.041874999999997</v>
       </c>
       <c r="L94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>26.658749999999998</v>
       </c>
       <c r="M94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>17.698125000000001</v>
       </c>
       <c r="N94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>5.5795624999999998</v>
       </c>
       <c r="O94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>54.419333333333327</v>
       </c>
       <c r="P94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>38.161999999999999</v>
       </c>
       <c r="Q94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>30.802000000000003</v>
       </c>
       <c r="R94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>24.142666666666663</v>
       </c>
       <c r="S94">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>16.201874999999998</v>
       </c>
     </row>
@@ -7990,63 +8386,63 @@
         <v>72.58064516129032</v>
       </c>
       <c r="D100">
-        <f t="shared" ref="D100:R100" si="23">ABS($B$98-D99)/($B$98)*100</f>
+        <f t="shared" ref="D100:R100" si="24">ABS($B$98-D99)/($B$98)*100</f>
         <v>3.2258064516129115</v>
       </c>
       <c r="E100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="F100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="G100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>6.4516129032258087</v>
       </c>
       <c r="H100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.6129032258064557</v>
       </c>
       <c r="I100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="J100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.6129032258064557</v>
       </c>
       <c r="K100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="L100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.6129032258064557</v>
       </c>
       <c r="M100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3.2258064516129115</v>
       </c>
       <c r="N100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.6129032258064557</v>
       </c>
       <c r="O100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="P100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>4.8387096774193541</v>
       </c>
       <c r="Q100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.6129032258064557</v>
       </c>
       <c r="R100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3.2258064516129115</v>
       </c>
     </row>
@@ -8263,76 +8659,76 @@
       </c>
     </row>
     <row r="105" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N105" s="102" t="s">
+      <c r="N105" s="152" t="s">
         <v>189</v>
       </c>
-      <c r="O105" s="102"/>
+      <c r="O105" s="152"/>
     </row>
     <row r="106" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B106" s="101" t="s">
+      <c r="B106" s="151" t="s">
         <v>228</v>
       </c>
-      <c r="C106" s="149"/>
-      <c r="D106" s="149"/>
-      <c r="E106" s="149"/>
-      <c r="F106" s="149"/>
-      <c r="G106" s="149"/>
-      <c r="H106" s="149"/>
-      <c r="I106" s="149"/>
-      <c r="J106" s="149"/>
-      <c r="K106" s="149"/>
-      <c r="N106" s="102"/>
-      <c r="O106" s="102"/>
+      <c r="C106" s="152"/>
+      <c r="D106" s="152"/>
+      <c r="E106" s="152"/>
+      <c r="F106" s="152"/>
+      <c r="G106" s="152"/>
+      <c r="H106" s="152"/>
+      <c r="I106" s="152"/>
+      <c r="J106" s="152"/>
+      <c r="K106" s="152"/>
+      <c r="N106" s="152"/>
+      <c r="O106" s="152"/>
     </row>
     <row r="107" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="101"/>
-      <c r="C107" s="149"/>
-      <c r="D107" s="149"/>
-      <c r="E107" s="149"/>
-      <c r="F107" s="149"/>
-      <c r="G107" s="149"/>
-      <c r="H107" s="149"/>
-      <c r="I107" s="149"/>
-      <c r="J107" s="149"/>
-      <c r="K107" s="149"/>
-      <c r="L107" s="153"/>
+      <c r="B107" s="151"/>
+      <c r="C107" s="152"/>
+      <c r="D107" s="152"/>
+      <c r="E107" s="152"/>
+      <c r="F107" s="152"/>
+      <c r="G107" s="152"/>
+      <c r="H107" s="152"/>
+      <c r="I107" s="152"/>
+      <c r="J107" s="152"/>
+      <c r="K107" s="152"/>
+      <c r="L107" s="1"/>
       <c r="N107" s="1"/>
     </row>
     <row r="108" spans="1:25" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="147" t="s">
+      <c r="B108" s="100" t="s">
         <v>217</v>
       </c>
-      <c r="C108" s="153" t="s">
+      <c r="C108" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D108" s="153" t="s">
+      <c r="D108" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E108" s="153" t="s">
+      <c r="E108" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F108" s="153" t="s">
+      <c r="F108" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G108" s="153" t="s">
+      <c r="G108" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H108" s="153" t="s">
+      <c r="H108" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="I108" s="153" t="s">
+      <c r="I108" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="J108" s="160" t="s">
+      <c r="J108" s="107" t="s">
         <v>225</v>
       </c>
-      <c r="K108" s="161" t="s">
+      <c r="K108" s="108" t="s">
         <v>226</v>
       </c>
-      <c r="L108" s="153" t="s">
+      <c r="L108" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="M108" s="162" t="s">
+      <c r="M108" s="1" t="s">
         <v>229</v>
       </c>
       <c r="N108" s="1" t="s">
@@ -8376,10 +8772,10 @@
       <c r="A109" s="73" t="s">
         <v>192</v>
       </c>
-      <c r="B109" s="153" t="s">
+      <c r="B109" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C109" s="147" t="s">
+      <c r="C109" s="100" t="s">
         <v>191</v>
       </c>
       <c r="D109" s="1" t="s">
@@ -8439,7 +8835,7 @@
       <c r="V109" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="W109" s="159" t="s">
+      <c r="W109" t="s">
         <v>213</v>
       </c>
       <c r="X109" s="1" t="s">
@@ -8453,31 +8849,31 @@
       <c r="A110" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B110" s="157">
+      <c r="B110" s="106">
         <v>2.4803E-4</v>
       </c>
-      <c r="C110" s="148">
+      <c r="C110" s="101">
         <v>2.4874000000000001E-4</v>
       </c>
-      <c r="D110" s="150">
+      <c r="D110" s="3">
         <v>2.5008000000000002E-4</v>
       </c>
-      <c r="E110" s="150">
+      <c r="E110" s="3">
         <v>1.6045E-4</v>
       </c>
-      <c r="F110" s="150">
+      <c r="F110" s="3">
         <v>2.5070000000000002E-4</v>
       </c>
-      <c r="G110" s="150">
+      <c r="G110" s="3">
         <v>2.4966000000000002E-4</v>
       </c>
-      <c r="H110" s="150">
+      <c r="H110" s="3">
         <v>2.5071000000000002E-4</v>
       </c>
-      <c r="I110" s="150">
+      <c r="I110" s="3">
         <v>2.5057999999999998E-4</v>
       </c>
-      <c r="J110" s="150">
+      <c r="J110" s="3">
         <v>2.5140999999999998E-4</v>
       </c>
       <c r="K110" s="3">
@@ -8492,10 +8888,10 @@
       <c r="N110" s="3">
         <v>1.6007E-4</v>
       </c>
-      <c r="O110" s="146">
+      <c r="O110">
         <v>-1.49E-2</v>
       </c>
-      <c r="P110" s="150">
+      <c r="P110" s="3">
         <v>-5.0571000000000001E-5</v>
       </c>
       <c r="Q110" s="3">
@@ -8530,45 +8926,38 @@
       <c r="A111" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B111" s="157"/>
-      <c r="C111" s="145"/>
-      <c r="D111" s="146"/>
-      <c r="E111" s="146"/>
-      <c r="F111" s="146"/>
-      <c r="G111" s="146"/>
-      <c r="H111" s="146"/>
-      <c r="I111" s="146"/>
-      <c r="J111" s="146"/>
+      <c r="B111" s="106"/>
+      <c r="C111" s="5"/>
     </row>
     <row r="112" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A112" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="B112" s="157">
+      <c r="B112" s="106">
         <v>2.4839000000000003E-4</v>
       </c>
-      <c r="C112" s="148">
+      <c r="C112" s="101">
         <v>2.4474000000000002E-4</v>
       </c>
-      <c r="D112" s="150">
+      <c r="D112" s="3">
         <v>1.4782E-4</v>
       </c>
-      <c r="E112" s="146">
+      <c r="E112">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="F112" s="150">
+      <c r="F112" s="3">
         <v>1.5220000000000001E-4</v>
       </c>
-      <c r="G112" s="150">
+      <c r="G112" s="3">
         <v>1.5088999999999999E-4</v>
       </c>
-      <c r="H112" s="150">
+      <c r="H112" s="3">
         <v>1.4833000000000001E-4</v>
       </c>
-      <c r="I112" s="150">
+      <c r="I112" s="3">
         <v>1.4949000000000001E-4</v>
       </c>
-      <c r="J112" s="150">
+      <c r="J112" s="3">
         <v>1.5154E-4</v>
       </c>
       <c r="K112" s="3">
@@ -8618,119 +9007,126 @@
       </c>
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A113" s="151" t="s">
+      <c r="A113" s="102" t="s">
         <v>197</v>
       </c>
-      <c r="B113" s="158">
+      <c r="B113" s="99">
         <f>ABS(B112/B110)*100</f>
         <v>100.14514373261301</v>
       </c>
-      <c r="C113" s="158">
-        <f t="shared" ref="C113:D113" si="24">ABS(C112/C110)*100</f>
+      <c r="C113" s="99">
+        <f t="shared" ref="C113:D113" si="25">ABS(C112/C110)*100</f>
         <v>98.391895151563887</v>
       </c>
-      <c r="D113" s="158">
-        <f t="shared" si="24"/>
+      <c r="D113" s="99">
+        <f t="shared" si="25"/>
         <v>59.109085092770307</v>
       </c>
-      <c r="E113" s="158">
+      <c r="E113" s="99">
         <f>ABS(E112/E110)*100</f>
         <v>4799.0028046120287</v>
       </c>
-      <c r="F113" s="158">
-        <f t="shared" ref="F113" si="25">ABS(F112/F110)*100</f>
+      <c r="F113" s="99">
+        <f t="shared" ref="F113" si="26">ABS(F112/F110)*100</f>
         <v>60.710011966493816</v>
       </c>
-      <c r="G113" s="158">
-        <f t="shared" ref="G113" si="26">ABS(G112/G110)*100</f>
+      <c r="G113" s="99">
+        <f t="shared" ref="G113" si="27">ABS(G112/G110)*100</f>
         <v>60.43819594648722</v>
       </c>
-      <c r="H113" s="158">
+      <c r="H113" s="99">
         <f>ABS(H112/H110)*100</f>
         <v>59.163974312951218</v>
       </c>
-      <c r="I113" s="158">
-        <f t="shared" ref="I113" si="27">ABS(I112/I110)*100</f>
+      <c r="I113" s="99">
+        <f t="shared" ref="I113" si="28">ABS(I112/I110)*100</f>
         <v>59.657594381036006</v>
       </c>
-      <c r="J113" s="158">
-        <f t="shared" ref="J113" si="28">ABS(J112/J110)*100</f>
+      <c r="J113" s="99">
+        <f t="shared" ref="J113" si="29">ABS(J112/J110)*100</f>
         <v>60.276043116821128</v>
       </c>
-      <c r="K113" s="158">
+      <c r="K113" s="99">
         <f>ABS(K112/K110)*100</f>
         <v>59.564261443134114</v>
       </c>
-      <c r="L113" s="158">
-        <f t="shared" ref="L113" si="29">ABS(L112/L110)*100</f>
+      <c r="L113" s="99">
+        <f t="shared" ref="L113" si="30">ABS(L112/L110)*100</f>
         <v>31.161156364797961</v>
       </c>
-      <c r="M113" s="158">
+      <c r="M113" s="99">
         <f>ABS(M112/M110)*100</f>
         <v>33.55596462443475</v>
       </c>
-      <c r="N113" s="158">
-        <f t="shared" ref="N113" si="30">ABS(N112/N110)*100</f>
+      <c r="N113" s="99">
+        <f t="shared" ref="N113" si="31">ABS(N112/N110)*100</f>
         <v>5497.5948022740058</v>
       </c>
-      <c r="O113" s="158">
-        <f t="shared" ref="O113" si="31">ABS(O112/O110)*100</f>
+      <c r="O113" s="99">
+        <f t="shared" ref="O113" si="32">ABS(O112/O110)*100</f>
         <v>1324.8322147651006</v>
       </c>
-      <c r="P113" s="158">
+      <c r="P113" s="99">
         <f>ABS(P112/P110)*100</f>
         <v>30056.75189337763</v>
       </c>
-      <c r="Q113" s="158">
-        <f t="shared" ref="Q113:R113" si="32">ABS(Q112/Q110)*100</f>
+      <c r="Q113" s="99">
+        <f t="shared" ref="Q113:R113" si="33">ABS(Q112/Q110)*100</f>
         <v>58.463127781309595</v>
       </c>
-      <c r="R113" s="158">
-        <f t="shared" si="32"/>
+      <c r="R113" s="99">
+        <f t="shared" si="33"/>
         <v>45.588822355289416</v>
       </c>
-      <c r="S113" s="158">
+      <c r="S113" s="99">
         <f>ABS(S112/S110)*100</f>
         <v>34.372679733343972</v>
       </c>
-      <c r="T113" s="158">
-        <f t="shared" ref="T113" si="33">ABS(T112/T110)*100</f>
+      <c r="T113" s="99">
+        <f t="shared" ref="T113" si="34">ABS(T112/T110)*100</f>
         <v>7838.0143696930108</v>
       </c>
-      <c r="U113" s="158">
-        <f t="shared" ref="U113" si="34">ABS(U112/U110)*100</f>
+      <c r="U113" s="99">
+        <f t="shared" ref="U113" si="35">ABS(U112/U110)*100</f>
         <v>1372.5579905751019</v>
       </c>
-      <c r="V113" s="158">
-        <f t="shared" ref="V113" si="35">ABS(V112/V110)*100</f>
+      <c r="V113" s="99">
+        <f t="shared" ref="V113" si="36">ABS(V112/V110)*100</f>
         <v>5561.1097225693575</v>
       </c>
-      <c r="W113" s="158">
-        <f t="shared" ref="W113" si="36">ABS(W112/W110)*100</f>
+      <c r="W113" s="99">
+        <f t="shared" ref="W113:Y113" si="37">ABS(W112/W110)*100</f>
         <v>34.992771084337356</v>
       </c>
-      <c r="X113" s="3"/>
+      <c r="X113" s="99">
+        <f t="shared" si="37"/>
+        <v>77.831747422064737</v>
+      </c>
+      <c r="Y113" s="99">
+        <f t="shared" si="37"/>
+        <v>40.032528814103856</v>
+      </c>
     </row>
     <row r="114" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A114" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B114" s="155"/>
-      <c r="C114" s="152"/>
-      <c r="D114" s="152"/>
-      <c r="E114" s="152"/>
-      <c r="F114" s="152"/>
-      <c r="G114" s="152"/>
-      <c r="H114" s="152"/>
-      <c r="I114" s="152"/>
-      <c r="J114" s="152"/>
-      <c r="K114" s="152"/>
+      <c r="B114" s="105"/>
+      <c r="C114" s="103"/>
+      <c r="D114" s="103"/>
+      <c r="E114" s="103"/>
+      <c r="F114" s="103"/>
+      <c r="G114" s="103"/>
+      <c r="H114" s="103"/>
+      <c r="I114" s="103"/>
+      <c r="J114" s="103"/>
+      <c r="K114" s="103"/>
     </row>
     <row r="115" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A115" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="B115" s="157">
+      <c r="B115" s="106">
         <v>2.4742999999999998E-4</v>
       </c>
       <c r="C115" s="3">
@@ -8807,13 +9203,13 @@
       <c r="A116" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B116" s="154"/>
+      <c r="B116" s="104"/>
     </row>
     <row r="117" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A117" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B117" s="157">
+      <c r="B117" s="106">
         <v>-4.9706000000000001E-4</v>
       </c>
       <c r="C117" s="3">
@@ -8890,7 +9286,7 @@
       <c r="A118" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B118" s="157">
+      <c r="B118" s="106">
         <v>9.9266000000000003E-4</v>
       </c>
       <c r="C118" s="3">
@@ -8963,27 +9359,14 @@
         <v>5.3804000000000005E-4</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B119" s="156"/>
-    </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B120" s="156"/>
-    </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B121" s="156"/>
-    </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="BI47:BN47"/>
-    <mergeCell ref="AX47:AZ47"/>
-    <mergeCell ref="AX57:AZ58"/>
-    <mergeCell ref="BA47:BC47"/>
-    <mergeCell ref="BA57:BC58"/>
-    <mergeCell ref="AP47:AR47"/>
-    <mergeCell ref="AP57:AR58"/>
-    <mergeCell ref="AU47:AW47"/>
-    <mergeCell ref="AU57:AW58"/>
-    <mergeCell ref="BD47:BG47"/>
+    <mergeCell ref="O72:S72"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="I72:N72"/>
+    <mergeCell ref="N105:O106"/>
+    <mergeCell ref="B106:K107"/>
     <mergeCell ref="A63:K63"/>
     <mergeCell ref="C10:N10"/>
     <mergeCell ref="E11:J11"/>
@@ -8995,12 +9378,16 @@
     <mergeCell ref="AC47:AF47"/>
     <mergeCell ref="AC46:AF46"/>
     <mergeCell ref="AG47:AO47"/>
-    <mergeCell ref="O72:S72"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="I72:N72"/>
-    <mergeCell ref="N105:O106"/>
-    <mergeCell ref="B106:K107"/>
+    <mergeCell ref="AP47:AR47"/>
+    <mergeCell ref="AP57:AR58"/>
+    <mergeCell ref="AU47:AW47"/>
+    <mergeCell ref="AU57:AW58"/>
+    <mergeCell ref="BD47:BG47"/>
+    <mergeCell ref="BI47:BN47"/>
+    <mergeCell ref="AX47:AZ47"/>
+    <mergeCell ref="AX57:AZ58"/>
+    <mergeCell ref="BA47:BC47"/>
+    <mergeCell ref="BA57:BC58"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C28:L28 C14:AD14">
@@ -9022,6 +9409,72 @@
         <color theme="9"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFC00000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C100:R100">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="9"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C76:S76">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="9"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C77:S77">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C80:S80">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="9"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C81:S81">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C84:S84">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="9"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -9229,73 +9682,216 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76:S76">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="9"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C84:S84">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="9"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C100:R100">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="9"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C77:S77">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="9"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C80:S80">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color theme="9"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C81:S81">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="9"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE245462-9E06-4DBC-B92A-835480425329}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440B9A49-A6D7-4F2F-BADF-5E0B97E19DDD}">
+  <dimension ref="A4:L35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="44" width="16.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4">
+        <v>2.4800000000000001E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B6" s="36">
+        <v>2.4890999999999997E-4</v>
+      </c>
+      <c r="C6" s="36">
+        <v>2.5150999999999998E-4</v>
+      </c>
+      <c r="D6" s="36">
+        <v>2.5084E-4</v>
+      </c>
+      <c r="E6" s="36">
+        <v>2.5075999999999999E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="154">
+        <f>ABS($B$4-B6)/($B$4)*100</f>
+        <v>0.36693548387095259</v>
+      </c>
+      <c r="C7" s="154">
+        <f t="shared" ref="C7:E7" si="0">ABS($B$4-C6)/($B$4)*100</f>
+        <v>1.4153225806451497</v>
+      </c>
+      <c r="D7" s="154">
+        <f t="shared" si="0"/>
+        <v>1.1451612903225779</v>
+      </c>
+      <c r="E7" s="154">
+        <f t="shared" si="0"/>
+        <v>1.1129032258064437</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8" s="36">
+        <v>2.4982999999999998E-4</v>
+      </c>
+      <c r="C8" s="36">
+        <v>2.0809999999999999E-4</v>
+      </c>
+      <c r="D8" s="36">
+        <v>1.6532E-4</v>
+      </c>
+      <c r="E8" s="36">
+        <v>9.8029000000000006E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" s="154">
+        <f>(B8/B6)*100</f>
+        <v>100.3696115061669</v>
+      </c>
+      <c r="C9" s="154">
+        <f t="shared" ref="C9:E9" si="1">(C8/C6)*100</f>
+        <v>82.740248896664141</v>
+      </c>
+      <c r="D9" s="154">
+        <f t="shared" si="1"/>
+        <v>65.906553978631806</v>
+      </c>
+      <c r="E9" s="154">
+        <f t="shared" si="1"/>
+        <v>39.092758015632484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B10" s="36">
+        <v>2.4844999999999999E-4</v>
+      </c>
+      <c r="C10" s="36">
+        <v>2.5049000000000002E-4</v>
+      </c>
+      <c r="D10" s="36">
+        <v>2.5040000000000001E-4</v>
+      </c>
+      <c r="E10" s="36">
+        <v>2.5040000000000001E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J28" s="153" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="152" t="s">
+        <v>243</v>
+      </c>
+      <c r="B35" s="152"/>
+      <c r="C35" s="152"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="152" t="s">
+        <v>244</v>
+      </c>
+      <c r="H35" s="152"/>
+      <c r="I35" s="152"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="A35:C35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1EEC65-86D5-47A4-BA26-302A87BD7670}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90CEC31-DCFA-4930-9151-A820B5EB4F0E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>